<commit_message>
Update to work live on the server
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol-Angel.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol-Angel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\Documents\Programming\SoftUni\JS-SPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\Documents\Programming\SoftUni\JS-SPA\JS-SPA-Ads-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -688,8 +688,8 @@
   </sheetPr>
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,7 +801,9 @@
       <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
@@ -820,7 +822,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="5">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>5</v>
@@ -832,7 +834,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="5">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>5</v>
@@ -844,7 +846,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
@@ -885,7 +887,9 @@
       <c r="D18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
@@ -1103,7 +1107,9 @@
       <c r="B37" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="7"/>
+      <c r="C37" s="7">
+        <v>0.2</v>
+      </c>
       <c r="D37" s="7" t="s">
         <v>28</v>
       </c>
@@ -1113,7 +1119,9 @@
       <c r="B38" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="7"/>
+      <c r="C38" s="7">
+        <v>0.2</v>
+      </c>
       <c r="D38" s="7" t="s">
         <v>28</v>
       </c>
@@ -1245,7 +1253,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C11:C50)</f>
-        <v>133</v>
+        <v>133.39999999999998</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>